<commit_message>
update readme and grading criterial
</commit_message>
<xml_diff>
--- a/Grading_Criterial.xlsx
+++ b/Grading_Criterial.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rioshi/Desktop/SADP-WWW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3D9E4E-7544-7342-AE84-78C08024A592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D2B1B-2679-2B42-A08B-0BA8FA17A4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19840" xr2:uid="{542EDA9B-4C27-A742-A9E1-8D84F295E3EB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19620" activeTab="4" xr2:uid="{542EDA9B-4C27-A742-A9E1-8D84F295E3EB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Case 1_PZ" sheetId="1" r:id="rId1"/>
+    <sheet name="Case 2_PR" sheetId="8" r:id="rId2"/>
+    <sheet name="Case 3_PA" sheetId="9" r:id="rId3"/>
+    <sheet name="Case 4_RM" sheetId="10" r:id="rId4"/>
+    <sheet name="Template" sheetId="12" r:id="rId5"/>
+    <sheet name="Weights" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="37">
   <si>
     <t>Adv</t>
   </si>
@@ -61,21 +65,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>Need</t>
-  </si>
-  <si>
-    <t>Not Need</t>
-  </si>
-  <si>
-    <t>Dynamic Multiple steps</t>
-  </si>
-  <si>
-    <t>Dynamic Two Steps</t>
-  </si>
-  <si>
-    <t>Static</t>
   </si>
   <si>
     <t>Impact Factor</t>
@@ -148,6 +137,24 @@
   <si>
     <t>Satisfied Decription
  (Select from drop list below)</t>
+  </si>
+  <si>
+    <t>Risk value w/o human</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>Weights</t>
   </si>
 </sst>
 </file>
@@ -549,143 +556,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7208D37D-F15E-CE40-964A-2E7D8A72846B}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="G1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="K1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H2" s="3"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="str">
-        <f>IF(C3="","",VLOOKUP(C3,Sheet2!A2:B4,2,FALSE))</f>
-        <v/>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <f>IF(C3="","",VLOOKUP(C3,Weights!A2:B4,2,FALSE))</f>
+        <v>0.9</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="str">
-        <f>IF(G3="Hard to detect",0.1,IF(G3="Easy to detect",0.9,""))</f>
-        <v/>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="str">
-        <f>IF(C4="","",VLOOKUP(C4,Sheet2!D2:E3,2,FALSE))</f>
-        <v/>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(C4="","",VLOOKUP(C4,Weights!D2:E3,2,FALSE))</f>
+        <v>0.5</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="str">
-        <f>IF(C5="","",VLOOKUP(C5,Sheet2!G2:H4,2,FALSE))</f>
-        <v/>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <f>IF(C5="","",VLOOKUP(C5,Weights!G2:H4,2,FALSE))</f>
+        <v>0.9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.4+D4*0.3+D5*0.3,""),""),"")</f>
-        <v/>
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.5+D4*0.3+D5*0.2,""),""),"")</f>
+        <v>0.78</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -693,10 +707,8 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -707,39 +719,35 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="1" t="str">
+      <c r="D8" s="1">
         <f>IF(D6&lt;&gt;"",1-D6,"")</f>
-        <v/>
+        <v>0.21999999999999997</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f>IF(H3="","",H3)</f>
-        <v/>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="1" t="str">
-        <f>IF(L3&lt;&gt;"",IF(L4&lt;&gt;"",IF(L5&lt;&gt;"",ROUND((IF(L3="yes",1,0)+IF(L4="yes",2,0)+IF(L5="yes",3,0))/6,2),""),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1">
+        <f>IF(G3="","",G3)</f>
+        <v>0.73</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <f>IF(J3&lt;&gt;"",IF(J4&lt;&gt;"",IF(J5&lt;&gt;"",IF(J3="yes",0.075,0)+IF(J4="yes",0.15,0)+IF(J5="yes",0.275,0),""),""),"")</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -750,10 +758,8 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -764,10 +770,8 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -778,34 +782,39 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f>IF(D8&lt;&gt;"",IF(H8&lt;&gt;"",IF(L8&lt;&gt;"",ROUND(((((D8-H8)*L8)+0.8)*6.25),1),""),""),"")</f>
-        <v/>
-      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((D8-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((0.5-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>2.7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
@@ -818,33 +827,33 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EAB8B87E-37D1-CB41-840E-01ACA2EB10A6}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$4</xm:f>
+            <xm:f>Weights!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C7315E04-6A67-8942-9DC9-AD6CB9A6CF2E}">
           <x14:formula1>
-            <xm:f>Sheet2!$D$2:$D$3</xm:f>
+            <xm:f>Weights!$D$2:$D$4</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4E9A481-B187-3348-BAF5-EED96C6A12BB}">
           <x14:formula1>
-            <xm:f>Sheet2!$G$2:$G$4</xm:f>
+            <xm:f>Weights!$G$2:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>C5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{28817776-30D2-834C-B76A-1111F63234D8}">
           <x14:formula1>
-            <xm:f>Sheet2!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G3</xm:sqref>
+            <xm:f>Weights!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{466761F9-57A5-D54B-95E2-2C8934D40899}">
           <x14:formula1>
-            <xm:f>Sheet2!$P$2:$P$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>L3:L5</xm:sqref>
+            <xm:f>Weights!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -853,14 +862,1226 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61534173-4D80-4E39-B993-5A85CF20FC04}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <f>IF(C3="","",VLOOKUP(C3,Weights!A2:B4,2,FALSE))</f>
+        <v>0.9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(C4="","",VLOOKUP(C4,Weights!D2:E4,2,FALSE))</f>
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <f>IF(C5="","",VLOOKUP(C5,Weights!G2:H4,2,FALSE))</f>
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.5+D4*0.3+D5*0.2,""),""),"")</f>
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1">
+        <f>IF(D6&lt;&gt;"",1-D6,"")</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1">
+        <f>IF(G3="","",G3)</f>
+        <v>0.18</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <f>IF(J3&lt;&gt;"",IF(J4&lt;&gt;"",IF(J5&lt;&gt;"",IF(J3="yes",0.075,0)+IF(J4="yes",0.15,0)+IF(J5="yes",0.275,0),""),""),"")</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((D8-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>3.1</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((0.5-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>4.8999999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EC4C2044-7543-477F-B3A3-36E6E8A0CF9D}">
+          <x14:formula1>
+            <xm:f>Weights!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AB9A3DB9-FEA1-433C-AEFA-5543AD2122D1}">
+          <x14:formula1>
+            <xm:f>Weights!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2214866D-1E94-4E8A-97D7-635EA86F3A05}">
+          <x14:formula1>
+            <xm:f>Weights!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D5AD503-58BB-4CF0-8539-480BF3399D30}">
+          <x14:formula1>
+            <xm:f>Weights!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99EF4AAB-F521-40F3-8DE9-C6F3A2720781}">
+          <x14:formula1>
+            <xm:f>Weights!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F775687D-097D-4F23-9A5B-4DB3EE88FC4D}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <f>IF(C3="","",VLOOKUP(C3,Weights!A2:B4,2,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(C4="","",VLOOKUP(C4,Weights!D2:E3,2,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <f>IF(C5="","",VLOOKUP(C5,Weights!G2:H4,2,FALSE))</f>
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.5+D4*0.3+D5*0.2,""),""),"")</f>
+        <v>0.18</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1">
+        <f>IF(D6&lt;&gt;"",1-D6,"")</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1">
+        <f>IF(G3="","",G3)</f>
+        <v>0.77</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <f>IF(J3&lt;&gt;"",IF(J4&lt;&gt;"",IF(J5&lt;&gt;"",IF(J3="yes",0.075,0)+IF(J4="yes",0.15,0)+IF(J5="yes",0.275,0),""),""),"")</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((D8-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>3.7</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((0.5-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F249542A-C41F-4ABE-9B7D-D4FDD59D6306}">
+          <x14:formula1>
+            <xm:f>Weights!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45573121-669C-4372-A112-DEE607D933C2}">
+          <x14:formula1>
+            <xm:f>Weights!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AD58BA9-69E4-4C52-8953-CB554B635300}">
+          <x14:formula1>
+            <xm:f>Weights!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{658C67B6-30ED-44A8-A4B2-2FC0E67C2DD6}">
+          <x14:formula1>
+            <xm:f>Weights!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B549079-5200-4E6E-A7AA-5F7843E01D25}">
+          <x14:formula1>
+            <xm:f>Weights!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381B12A0-8C77-4D14-833E-114542D9922F}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <f>IF(C3="","",VLOOKUP(C3,Weights!A2:B4,2,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(C4="","",VLOOKUP(C4,Weights!D2:E3,2,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <f>IF(C5="","",VLOOKUP(C5,Weights!G2:H4,2,FALSE))</f>
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.5+D4*0.3+D5*0.2,""),""),"")</f>
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1">
+        <f>IF(D6&lt;&gt;"",1-D6,"")</f>
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1">
+        <f>IF(G3="","",G3)</f>
+        <v>0.18</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <f>IF(J3&lt;&gt;"",IF(J4&lt;&gt;"",IF(J5&lt;&gt;"",IF(J3="yes",0.075,0)+IF(J4="yes",0.15,0)+IF(J5="yes",0.275,0),""),""),"")</f>
+        <v>0.35000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((D8-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>8.2999999999999989</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((0.5-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v>6.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F2C16FBB-CBAB-4974-BB14-93B2B4E82344}">
+          <x14:formula1>
+            <xm:f>Weights!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6CABD77A-711F-42B0-8922-0A971119EEDF}">
+          <x14:formula1>
+            <xm:f>Weights!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D706991D-3EE4-4F54-B9FA-19035DEBF55B}">
+          <x14:formula1>
+            <xm:f>Weights!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9795A5CF-E9DA-4077-8BD4-A409CB266CB3}">
+          <x14:formula1>
+            <xm:f>Weights!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B528B79-3F84-422D-B54B-B2C4F8AD16FD}">
+          <x14:formula1>
+            <xm:f>Weights!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904434C1-A551-044B-B085-4365ACBEB0EF}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="str">
+        <f>IF(C3="","",VLOOKUP(C3,Weights!A2:B4,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="str">
+        <f>IF(C4="","",VLOOKUP(C4,Weights!D2:E3,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="str">
+        <f>IF(C5="","",VLOOKUP(C5,Weights!G2:H4,2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>IF(D3&lt;&gt;"",IF(D4&lt;&gt;"",IF(D5&lt;&gt;"",D3*0.5+D4*0.3+D5*0.2,""),""),"")</f>
+        <v/>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="str">
+        <f>IF(D6&lt;&gt;"",1-D6,"")</f>
+        <v/>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>IF(G3="","",G3)</f>
+        <v/>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f>IF(J3&lt;&gt;"",IF(J4&lt;&gt;"",IF(J5&lt;&gt;"",IF(J3="yes",0.075,0)+IF(J4="yes",0.15,0)+IF(J5="yes",0.275,0),""),""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((D8-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v/>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f>IF(D8&lt;&gt;"",IF(G8&lt;&gt;"",IF(J8&lt;&gt;"",ROUNDUP((((0.5-G8+0.8)*(1+J8))*4),1),""),""),"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{820FB85B-65D6-F341-9D88-E2692AB77BAF}">
+          <x14:formula1>
+            <xm:f>Weights!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80CBFB5F-D0AA-0B4D-91F5-39BC6170446C}">
+          <x14:formula1>
+            <xm:f>Weights!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF69BDDD-8386-4C40-B095-A0C39FE4A716}">
+          <x14:formula1>
+            <xm:f>Weights!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71ECB6F4-5C39-D545-BF29-C7774C19B0F7}">
+          <x14:formula1>
+            <xm:f>Weights!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0A306BAA-5AFE-7441-8F5F-B3BBECC3769D}">
+          <x14:formula1>
+            <xm:f>Weights!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B029510E-03EE-7F49-9213-4E07F06D4058}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
@@ -888,54 +2109,54 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0.1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>0.1</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>0.1</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -946,54 +2167,129 @@
         <v>0.5</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>0.5</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <v>0.9</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>0.15</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0.9</v>
       </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0.9</v>
+      </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>0.9</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N4">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>0.27500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Additional information in Readme and excel
</commit_message>
<xml_diff>
--- a/Grading_Criterial.xlsx
+++ b/Grading_Criterial.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rioshi/Desktop/SADP-WWW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rioshi/Desktop/Decoding-Deceptive-Patterns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D2B1B-2679-2B42-A08B-0BA8FA17A4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651C83B1-3884-0F4D-888D-4EF61844164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19620" activeTab="4" xr2:uid="{542EDA9B-4C27-A742-A9E1-8D84F295E3EB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19640" activeTab="4" xr2:uid="{542EDA9B-4C27-A742-A9E1-8D84F295E3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Case 1_PZ" sheetId="1" r:id="rId1"/>
     <sheet name="Case 2_PR" sheetId="8" r:id="rId2"/>
     <sheet name="Case 3_PA" sheetId="9" r:id="rId3"/>
     <sheet name="Case 4_RM" sheetId="10" r:id="rId4"/>
-    <sheet name="Template" sheetId="12" r:id="rId5"/>
-    <sheet name="Weights" sheetId="2" r:id="rId6"/>
+    <sheet name="…..." sheetId="13" r:id="rId5"/>
+    <sheet name="Template" sheetId="12" r:id="rId6"/>
+    <sheet name="Weights" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
   <si>
     <t>Adv</t>
   </si>
@@ -155,19 +156,28 @@
   </si>
   <si>
     <t>Weights</t>
+  </si>
+  <si>
+    <t>More Case Study will be released
+Soon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,6 +231,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,7 +572,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:J14"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1118,15 +1131,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1425,15 +1438,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1732,15 +1745,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1783,10 +1796,225 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFAEE35D-BC31-B74B-B4CC-03C25153706C}">
+  <dimension ref="G14:S26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="14" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+    </row>
+    <row r="17" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="19" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+    </row>
+    <row r="21" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+    </row>
+    <row r="25" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+    </row>
+    <row r="26" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G14:S26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904434C1-A551-044B-B085-4365ACBEB0EF}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -2023,15 +2251,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2073,7 +2301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B029510E-03EE-7F49-9213-4E07F06D4058}">
   <dimension ref="A1:P18"/>
   <sheetViews>

</xml_diff>